<commit_message>
Se hace la planeacion de la iteracion 3
</commit_message>
<xml_diff>
--- a/Plantillas/Iteracion 2/Plantilla Lista de Tareas de la Iteracion.xlsx
+++ b/Plantillas/Iteracion 2/Plantilla Lista de Tareas de la Iteracion.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enriq\Documents\6TO SEMESTRE IS\DESARROLLO SOFTWARE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enriq\Documents\6TO SEMESTRE IS\DESARROLLO SOFTWARE\Proyecto\EMA-Desarrollo-de-software-Equipo-2\Plantillas\Iteracion 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -867,7 +867,7 @@
       <pane xSplit="6" ySplit="5" topLeftCell="L107" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="BB114" sqref="BB114"/>
+      <selection pane="bottomRight" activeCell="A117" sqref="A117:XFD117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16551,7 +16551,7 @@
       </c>
       <c r="BB114" s="13">
         <f>SUM(AZ114:AZ119)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115" spans="1:54" s="13" customFormat="1" ht="46.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
@@ -16846,7 +16846,7 @@
         <v>92</v>
       </c>
       <c r="F117" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G117" s="15">
         <v>1</v>
@@ -16867,10 +16867,12 @@
         <v>1</v>
       </c>
       <c r="M117" s="16"/>
-      <c r="N117" s="16"/>
+      <c r="N117" s="16">
+        <v>1</v>
+      </c>
       <c r="O117" s="16">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P117" s="16"/>
       <c r="Q117" s="16">
@@ -16878,7 +16880,7 @@
       </c>
       <c r="R117" s="16">
         <f t="shared" si="36"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S117" s="16"/>
       <c r="T117" s="16">
@@ -16886,7 +16888,7 @@
       </c>
       <c r="U117" s="16">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V117" s="16"/>
       <c r="W117" s="16">
@@ -16894,13 +16896,13 @@
       </c>
       <c r="X117" s="16">
         <f t="shared" si="38"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y117" s="16"/>
       <c r="Z117" s="16"/>
       <c r="AA117" s="16">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB117" s="16"/>
       <c r="AC117" s="16">
@@ -16908,7 +16910,7 @@
       </c>
       <c r="AD117" s="16">
         <f t="shared" si="40"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE117" s="16"/>
       <c r="AF117" s="16">
@@ -16916,7 +16918,7 @@
       </c>
       <c r="AG117" s="16">
         <f t="shared" si="41"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH117" s="16"/>
       <c r="AI117" s="16">
@@ -16924,7 +16926,7 @@
       </c>
       <c r="AJ117" s="16">
         <f t="shared" si="42"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK117" s="16"/>
       <c r="AL117" s="16">
@@ -16932,7 +16934,7 @@
       </c>
       <c r="AM117" s="16">
         <f t="shared" si="43"/>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="AN117" s="16"/>
       <c r="AO117" s="16">
@@ -16940,7 +16942,7 @@
       </c>
       <c r="AP117" s="16">
         <f t="shared" si="44"/>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="AQ117" s="16"/>
       <c r="AR117" s="16">
@@ -16948,7 +16950,7 @@
       </c>
       <c r="AS117" s="16">
         <f t="shared" si="45"/>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="AT117" s="16"/>
       <c r="AU117" s="16">
@@ -16956,21 +16958,21 @@
       </c>
       <c r="AV117" s="16">
         <f t="shared" si="46"/>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="AW117" s="16"/>
       <c r="AX117" s="16"/>
       <c r="AY117" s="16">
         <f t="shared" si="47"/>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="AZ117" s="16">
         <f t="shared" si="54"/>
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="BA117" s="16">
         <f t="shared" si="48"/>
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="118" spans="1:54" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -18691,11 +18693,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AZ4:BA4"/>
-    <mergeCell ref="AO4:AP4"/>
-    <mergeCell ref="AR4:AS4"/>
-    <mergeCell ref="AU4:AV4"/>
-    <mergeCell ref="AX4:AY4"/>
     <mergeCell ref="AL4:AM4"/>
     <mergeCell ref="H4:I4"/>
     <mergeCell ref="K4:L4"/>
@@ -18707,6 +18704,11 @@
     <mergeCell ref="AC4:AD4"/>
     <mergeCell ref="AF4:AG4"/>
     <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AZ4:BA4"/>
+    <mergeCell ref="AO4:AP4"/>
+    <mergeCell ref="AR4:AS4"/>
+    <mergeCell ref="AU4:AV4"/>
+    <mergeCell ref="AX4:AY4"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.62992125984251968" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>